<commit_message>
training only on Sixray, while gun is an anomaly
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dndlssardar\OneDrive - Smiths Group\Documents\Soumen\skip-ganomaly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E53A204-A12E-4C0D-ABC6-D3DFA8F20C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9871BE36-873D-4E51-9D52-1D4D74DEAB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6408" yWindow="1512" windowWidth="15432" windowHeight="10728" xr2:uid="{CC5E58DF-02CC-4751-A82B-FC0F51D22954}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CC5E58DF-02CC-4751-A82B-FC0F51D22954}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Experiment Description</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>nc</t>
+  </si>
+  <si>
+    <t>exp5_sixraysd3_ep75_nc1_px64_traycrop_gun</t>
+  </si>
+  <si>
+    <t>sixraysd3_nc1_px64_traycrop_gun</t>
+  </si>
+  <si>
+    <t>Experiment Name</t>
+  </si>
+  <si>
+    <t>sixray_sd3_grey_exp_px64</t>
+  </si>
+  <si>
+    <t>sixray_sd3_greyscale_50epoch</t>
   </si>
 </sst>
 </file>
@@ -152,10 +167,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -173,6 +191,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>17930</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>2366683</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1215601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F8D9319-6F28-4FDA-9EAC-6B68794CD076}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9502589" y="5136777"/>
+          <a:ext cx="2348753" cy="1170777"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -472,183 +539,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D0CBE7-A61F-4A8E-A7D2-07FFFF8AB171}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>256</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
       </c>
       <c r="I2" t="s">
         <v>5</v>
       </c>
       <c r="J2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>256</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
       </c>
       <c r="I3" t="s">
         <v>5</v>
       </c>
       <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>64</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>50</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
       </c>
       <c r="J4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>64</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>50</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>64</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>75</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>